<commit_message>
updating the proposal and CBA
</commit_message>
<xml_diff>
--- a/Systems' CBA.xlsx
+++ b/Systems' CBA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eyad2\Desktop\AEOA_Project1_SAD_20232024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5BD4B1-CF64-4B65-8B7F-43E68017582D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D40CC16-4CC8-4CE5-8363-411F3B6568C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10580" yWindow="710" windowWidth="10710" windowHeight="9970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -637,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="89" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -676,11 +676,11 @@
         <v>6</v>
       </c>
       <c r="C6" s="1">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="D6" s="10">
         <f xml:space="preserve"> C6</f>
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="H6" s="4"/>
     </row>
@@ -689,11 +689,11 @@
         <v>7</v>
       </c>
       <c r="C7" s="1">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="D7" s="10">
         <f xml:space="preserve"> C7</f>
-        <v>0</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
@@ -701,11 +701,11 @@
         <v>19</v>
       </c>
       <c r="C8" s="1">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="D8" s="10">
         <f xml:space="preserve"> C8</f>
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
@@ -713,10 +713,11 @@
         <v>8</v>
       </c>
       <c r="C9" s="1">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="D9" s="10">
-        <v>10000</v>
+        <f xml:space="preserve"> C9</f>
+        <v>5000</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
@@ -725,10 +726,11 @@
         <v>20</v>
       </c>
       <c r="C10" s="1">
-        <v>20000</v>
+        <v>7500</v>
       </c>
       <c r="D10" s="10">
-        <v>20000</v>
+        <f xml:space="preserve"> C10</f>
+        <v>7500</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
@@ -738,7 +740,7 @@
       <c r="C11" s="28"/>
       <c r="D11" s="2">
         <f xml:space="preserve"> D6 + D7 + D8 + D9 + D10</f>
-        <v>50000</v>
+        <v>47500</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.35">
@@ -852,15 +854,15 @@
       <c r="D18" s="17"/>
       <c r="E18" s="17">
         <f xml:space="preserve"> D11 + E17</f>
-        <v>68750</v>
+        <v>66250</v>
       </c>
       <c r="F18" s="25">
         <f xml:space="preserve"> E18 + F17</f>
-        <v>84375</v>
+        <v>81875</v>
       </c>
       <c r="G18" s="25">
         <f>F18 + G17</f>
-        <v>95949.074074074073</v>
+        <v>93449.074074074073</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -986,15 +988,15 @@
       </c>
       <c r="E27" s="4">
         <f>E26 - E18</f>
-        <v>-6250</v>
+        <v>-3750</v>
       </c>
       <c r="F27" s="4">
         <f xml:space="preserve"> F26 - F18</f>
-        <v>30208.333333333328</v>
+        <v>32708.333333333328</v>
       </c>
       <c r="G27" s="4">
         <f xml:space="preserve"> G26 - G18</f>
-        <v>62037.037037037051</v>
+        <v>64537.037037037051</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.35">
@@ -1004,7 +1006,7 @@
       <c r="C28" s="3"/>
       <c r="D28" s="6">
         <f xml:space="preserve"> G27 / D11</f>
-        <v>1.2407407407407409</v>
+        <v>1.358674463937622</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.35">

</xml_diff>